<commit_message>
mostly finish algorithm analysis
</commit_message>
<xml_diff>
--- a/misc/Graphs.xlsx
+++ b/misc/Graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Documents\School\OS\ConcurrencySolutions\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09E0B9FC-D326-411F-9E4A-57D39BB2BEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{683B6B49-E2DD-4FDB-A957-D6E7D8B836B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A2843F0-0F36-47B8-9E50-9B4C825E4008}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0A2843F0-0F36-47B8-9E50-9B4C825E4008}"/>
   </bookViews>
   <sheets>
     <sheet name="Algorithm 2, 4 Philosophers" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="9">
   <si>
     <t>Philosopher 1</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Std dev</t>
+  </si>
+  <si>
+    <t>Total clocks</t>
   </si>
 </sst>
 </file>
@@ -5859,10 +5862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89CB6333-8F62-450A-B33E-CCB76B8BF0D4}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6170,7 +6173,7 @@
         <v>7288.75</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:E22" si="0">AVERAGE(B2:B21)</f>
+        <f t="shared" ref="B22:D22" si="0">AVERAGE(B2:B21)</f>
         <v>10218.200000000001</v>
       </c>
       <c r="C22">
@@ -6237,6 +6240,31 @@
       </c>
       <c r="F24" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>SUM(A2:A21)</f>
+        <v>145775</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:D25" si="3">SUM(B2:B21)</f>
+        <v>204364</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>161143</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="3"/>
+        <v>130867</v>
+      </c>
+      <c r="E25">
+        <f>SUM(A2:D21)</f>
+        <v>642149</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -6248,10 +6276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9865F81-9FD2-4737-A99C-90857E4FDF4C}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22:G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6703,6 +6731,35 @@
         <v>7</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>SUM(A2:A21)</f>
+        <v>110575</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:E25" si="3">SUM(B2:B21)</f>
+        <v>143810</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>180704</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="3"/>
+        <v>156837</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>154854</v>
+      </c>
+      <c r="F25">
+        <f>SUM(A2:E21)</f>
+        <v>746780</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6712,10 +6769,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE14E76-CBDC-4F26-8B4C-EDEC6DEB6273}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="A25" sqref="A25:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7092,6 +7149,31 @@
         <v>7</v>
       </c>
     </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>SUM(A2:A21)</f>
+        <v>113003</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:D25" si="3">SUM(B2:B21)</f>
+        <v>119533</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>115349</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="3"/>
+        <v>128427</v>
+      </c>
+      <c r="E25">
+        <f>SUM(A2:D21)</f>
+        <v>476312</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7100,10 +7182,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280DC659-8C04-47AF-937F-7C62D538C7C0}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="A25" sqref="A25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7555,6 +7637,35 @@
         <v>7</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>SUM(A2:A21)</f>
+        <v>177146</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:E25" si="3">SUM(B2:B21)</f>
+        <v>121337</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>129600</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="3"/>
+        <v>167875</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>160760</v>
+      </c>
+      <c r="F25">
+        <f>SUM(A2:E21)</f>
+        <v>756718</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7562,6 +7673,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="223f284c-d283-496d-bc9d-bf628f5c0687" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100715311BB098BB947B40B1D10EC700E62" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c178c0888a048e8aa43d8bb6bab666af">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="223f284c-d283-496d-bc9d-bf628f5c0687" xmlns:ns4="405b48d2-7906-4226-9687-8714d50f51b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0583250fcfb1fac2bab5e8965dfd61c" ns3:_="" ns4:_="">
     <xsd:import namespace="223f284c-d283-496d-bc9d-bf628f5c0687"/>
@@ -7808,24 +7936,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89E9F1B0-89BD-48FA-8C67-067224EA1409}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="405b48d2-7906-4226-9687-8714d50f51b9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="223f284c-d283-496d-bc9d-bf628f5c0687"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="223f284c-d283-496d-bc9d-bf628f5c0687" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52754233-6ACC-4D29-BC99-600CE1EC357C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B71E6A0F-3861-46E1-A8A4-0F1844A6381F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7842,29 +7978,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52754233-6ACC-4D29-BC99-600CE1EC357C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89E9F1B0-89BD-48FA-8C67-067224EA1409}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="405b48d2-7906-4226-9687-8714d50f51b9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="223f284c-d283-496d-bc9d-bf628f5c0687"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>